<commit_message>
updated courts template (#646)
Co-authored-by: Michelle Orden <michelleorden@michelles-mbp.lan>
</commit_message>
<xml_diff>
--- a/publisher/public/assets/COURTS_AND_PRETRIAL.xlsx
+++ b/publisher/public/assets/COURTS_AND_PRETRIAL.xlsx
@@ -24,14 +24,13 @@
     <sheet name="cases_filed" sheetId="15" r:id="rId15"/>
     <sheet name="cases_filed_by_severity" sheetId="16" r:id="rId16"/>
     <sheet name="offenses_on_release" sheetId="17" r:id="rId17"/>
-    <sheet name="cases_overturned" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3857" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="93">
   <si>
     <t>year</t>
   </si>
@@ -12947,40 +12946,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>

</xml_diff>